<commit_message>
Something went terribly wrong here
</commit_message>
<xml_diff>
--- a/data/motorEnergy_shares.xlsx
+++ b/data/motorEnergy_shares.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Box/BATMAN/Coding/Battery_replacements/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Box/BATMAN/Coding/product_component_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44D473B-53C4-7E48-A578-AD14375DD7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A22942-8938-F447-A393-053B80C2C733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="31080" windowHeight="20760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -472,7 +472,7 @@
         <v>2011</v>
       </c>
       <c r="D2">
-        <v>3.5989952976177371E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>